<commit_message>
Add VRayLightMtl && CoronaLightMtl
</commit_message>
<xml_diff>
--- a/RedHaloM2B_Lib/ParamBlock2/PB2.xlsx
+++ b/RedHaloM2B_Lib/ParamBlock2/PB2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APP\RedHaloM2B_Lib\RedHaloM2B_Lib\ParamBlock2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2F4CC6-CF40-4740-8CBE-17276B87C60B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02AA4D8-1C27-4D57-B5E2-0F03DA376407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13875" yWindow="3990" windowWidth="27105" windowHeight="13710" tabRatio="706" firstSheet="21" activeTab="28" xr2:uid="{3B29243F-53F5-4745-B8C6-E4F7709AB902}"/>
+    <workbookView xWindow="51480" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="706" firstSheet="23" activeTab="29" xr2:uid="{3B29243F-53F5-4745-B8C6-E4F7709AB902}"/>
   </bookViews>
   <sheets>
     <sheet name="Checker" sheetId="6" r:id="rId1"/>
@@ -43,6 +43,8 @@
     <sheet name="StandardMtl" sheetId="29" r:id="rId28"/>
     <sheet name="VRayCarPaintMtl2" sheetId="30" r:id="rId29"/>
     <sheet name="Color Map (22)" sheetId="32" r:id="rId30"/>
+    <sheet name="Color Map (23)" sheetId="33" r:id="rId31"/>
+    <sheet name="Color Map (24)" sheetId="34" r:id="rId32"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Bitmap!#REF!</definedName>
@@ -50,6 +52,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Color Correction'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Color Map'!$A$2:$A$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="29" hidden="1">'Color Map (22)'!$A$2:$A$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="30" hidden="1">'Color Map (23)'!$A$2:$A$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="31" hidden="1">'Color Map (24)'!$A$2:$A$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">Composite!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">CoronaAO!$A$2:$A$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">CoronaBumpConverter!$A$2:$A$4</definedName>
@@ -86,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="899">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2248" uniqueCount="899">
   <si>
     <t>soften</t>
   </si>
@@ -3001,7 +3005,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3059,14 +3063,103 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="187">
+  <dxfs count="199">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <name val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <name val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4800,202 +4893,202 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4060F31A-9C61-4466-9687-2436457AD7E4}" name="表2" displayName="表2" ref="A2:D18" totalsRowShown="0" headerRowDxfId="186" headerRowBorderDxfId="185" tableBorderDxfId="184" totalsRowBorderDxfId="183">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4060F31A-9C61-4466-9687-2436457AD7E4}" name="表2" displayName="表2" ref="A2:D18" totalsRowShown="0" headerRowDxfId="198" headerRowBorderDxfId="197" tableBorderDxfId="196" totalsRowBorderDxfId="195">
   <autoFilter ref="A2:D18" xr:uid="{4060F31A-9C61-4466-9687-2436457AD7E4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{2D41582E-7698-4D96-B381-E70F10A1DC8F}" name="main" dataDxfId="182"/>
-    <tableColumn id="2" xr3:uid="{251B123A-D391-4C42-A03C-DDA697EA139B}" name="branch" dataDxfId="181"/>
-    <tableColumn id="3" xr3:uid="{A937446C-F8DF-404A-8C19-2C649D8F1BEB}" name="type" dataDxfId="180"/>
-    <tableColumn id="4" xr3:uid="{206B0CBC-2C23-4005-9413-91FFD450242E}" name="param name" dataDxfId="179"/>
+    <tableColumn id="1" xr3:uid="{2D41582E-7698-4D96-B381-E70F10A1DC8F}" name="main" dataDxfId="194"/>
+    <tableColumn id="2" xr3:uid="{251B123A-D391-4C42-A03C-DDA697EA139B}" name="branch" dataDxfId="193"/>
+    <tableColumn id="3" xr3:uid="{A937446C-F8DF-404A-8C19-2C649D8F1BEB}" name="type" dataDxfId="192"/>
+    <tableColumn id="4" xr3:uid="{206B0CBC-2C23-4005-9413-91FFD450242E}" name="param name" dataDxfId="191"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D88250FB-0DB3-424D-A24A-D8261708B2E3}" name="表6_892" displayName="表6_892" ref="A1:D46" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D88250FB-0DB3-424D-A24A-D8261708B2E3}" name="表6_892" displayName="表6_892" ref="A1:D46" totalsRowShown="0" headerRowDxfId="137" dataDxfId="136">
   <autoFilter ref="A1:D46" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{ABC109BE-05F7-45FC-B28E-A25F56785127}" name="main" dataDxfId="123"/>
-    <tableColumn id="2" xr3:uid="{98C68B2C-8456-453F-ABDC-E94E9B8D474D}" name="branch" dataDxfId="122"/>
-    <tableColumn id="3" xr3:uid="{73ACFFB3-7807-4088-807D-88470729B2BA}" name="type" dataDxfId="121"/>
-    <tableColumn id="4" xr3:uid="{320F409E-253F-4260-8467-E0D287495D07}" name="param name" dataDxfId="120"/>
+    <tableColumn id="1" xr3:uid="{ABC109BE-05F7-45FC-B28E-A25F56785127}" name="main" dataDxfId="135"/>
+    <tableColumn id="2" xr3:uid="{98C68B2C-8456-453F-ABDC-E94E9B8D474D}" name="branch" dataDxfId="134"/>
+    <tableColumn id="3" xr3:uid="{73ACFFB3-7807-4088-807D-88470729B2BA}" name="type" dataDxfId="133"/>
+    <tableColumn id="4" xr3:uid="{320F409E-253F-4260-8467-E0D287495D07}" name="param name" dataDxfId="132"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{C4B0AB83-5BB3-4AD6-9F5A-8C690B2DA3FE}" name="表6_89212" displayName="表6_89212" ref="A1:D13" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{C4B0AB83-5BB3-4AD6-9F5A-8C690B2DA3FE}" name="表6_89212" displayName="表6_89212" ref="A1:D13" totalsRowShown="0" headerRowDxfId="131" dataDxfId="130">
   <autoFilter ref="A1:D13" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{25807113-C158-42E7-8892-EDA341B2D700}" name="main" dataDxfId="117"/>
-    <tableColumn id="2" xr3:uid="{821DBFB3-8F0C-4625-9C08-E53307BC75E4}" name="branch" dataDxfId="116"/>
-    <tableColumn id="3" xr3:uid="{9138AA34-C209-41F6-A065-D789CE7DFF08}" name="type" dataDxfId="115"/>
-    <tableColumn id="4" xr3:uid="{FBACDFD2-4E34-4DC7-99FF-33D8FF23E785}" name="param name" dataDxfId="114"/>
+    <tableColumn id="1" xr3:uid="{25807113-C158-42E7-8892-EDA341B2D700}" name="main" dataDxfId="129"/>
+    <tableColumn id="2" xr3:uid="{821DBFB3-8F0C-4625-9C08-E53307BC75E4}" name="branch" dataDxfId="128"/>
+    <tableColumn id="3" xr3:uid="{9138AA34-C209-41F6-A065-D789CE7DFF08}" name="type" dataDxfId="127"/>
+    <tableColumn id="4" xr3:uid="{FBACDFD2-4E34-4DC7-99FF-33D8FF23E785}" name="param name" dataDxfId="126"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{753F4B04-15DB-4DDB-B21D-C7A8F3C7E798}" name="表6_8921213" displayName="表6_8921213" ref="A1:D5" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{753F4B04-15DB-4DDB-B21D-C7A8F3C7E798}" name="表6_8921213" displayName="表6_8921213" ref="A1:D5" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124">
   <autoFilter ref="A1:D5" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BB4AA73D-1ED5-448B-9AE3-FE865C983D39}" name="main" dataDxfId="111"/>
-    <tableColumn id="2" xr3:uid="{EB99AB73-8FDC-45BF-B0A0-8377793F09C3}" name="branch" dataDxfId="110"/>
-    <tableColumn id="3" xr3:uid="{991EAF0A-5DA2-439D-9FAB-9DEFD89077A0}" name="type" dataDxfId="109"/>
-    <tableColumn id="4" xr3:uid="{D18C9DB0-8246-4734-A938-2CB4F7229F15}" name="param name" dataDxfId="108"/>
+    <tableColumn id="1" xr3:uid="{BB4AA73D-1ED5-448B-9AE3-FE865C983D39}" name="main" dataDxfId="123"/>
+    <tableColumn id="2" xr3:uid="{EB99AB73-8FDC-45BF-B0A0-8377793F09C3}" name="branch" dataDxfId="122"/>
+    <tableColumn id="3" xr3:uid="{991EAF0A-5DA2-439D-9FAB-9DEFD89077A0}" name="type" dataDxfId="121"/>
+    <tableColumn id="4" xr3:uid="{D18C9DB0-8246-4734-A938-2CB4F7229F15}" name="param name" dataDxfId="120"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{A24E004E-4EBE-490C-9AAB-ED6960D629C9}" name="表6_892121314" displayName="表6_892121314" ref="A1:D4" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{A24E004E-4EBE-490C-9AAB-ED6960D629C9}" name="表6_892121314" displayName="表6_892121314" ref="A1:D4" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118">
   <autoFilter ref="A1:D4" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DA2F9135-19FD-41FF-A0BD-E19EDE35978C}" name="main" dataDxfId="105"/>
-    <tableColumn id="2" xr3:uid="{9A0AF032-2605-41F3-87D5-7A2191868ADF}" name="branch" dataDxfId="104"/>
-    <tableColumn id="3" xr3:uid="{39447203-25E4-4E57-BB37-9154C8CD7663}" name="type" dataDxfId="103"/>
-    <tableColumn id="4" xr3:uid="{BF6E1539-2F98-444C-9F1B-1DD9890B3898}" name="param name" dataDxfId="102"/>
+    <tableColumn id="1" xr3:uid="{DA2F9135-19FD-41FF-A0BD-E19EDE35978C}" name="main" dataDxfId="117"/>
+    <tableColumn id="2" xr3:uid="{9A0AF032-2605-41F3-87D5-7A2191868ADF}" name="branch" dataDxfId="116"/>
+    <tableColumn id="3" xr3:uid="{39447203-25E4-4E57-BB37-9154C8CD7663}" name="type" dataDxfId="115"/>
+    <tableColumn id="4" xr3:uid="{BF6E1539-2F98-444C-9F1B-1DD9890B3898}" name="param name" dataDxfId="114"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{64A915F8-A0A7-42F8-B358-548E26A2D261}" name="表6_89212131415" displayName="表6_89212131415" ref="A1:D14" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{64A915F8-A0A7-42F8-B358-548E26A2D261}" name="表6_89212131415" displayName="表6_89212131415" ref="A1:D14" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
   <autoFilter ref="A1:D14" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{AE618ED7-34F9-45C9-BA6E-0E28742D773C}" name="main" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{B312A00E-85C1-49DD-9CE3-820C1CB05E6B}" name="branch" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{2EB76E35-76BD-4322-995B-7CC45A5F5D7F}" name="type" dataDxfId="97"/>
-    <tableColumn id="4" xr3:uid="{2C20F636-3553-402B-A09E-80722A9BC84D}" name="param name" dataDxfId="96"/>
+    <tableColumn id="1" xr3:uid="{AE618ED7-34F9-45C9-BA6E-0E28742D773C}" name="main" dataDxfId="111"/>
+    <tableColumn id="2" xr3:uid="{B312A00E-85C1-49DD-9CE3-820C1CB05E6B}" name="branch" dataDxfId="110"/>
+    <tableColumn id="3" xr3:uid="{2EB76E35-76BD-4322-995B-7CC45A5F5D7F}" name="type" dataDxfId="109"/>
+    <tableColumn id="4" xr3:uid="{2C20F636-3553-402B-A09E-80722A9BC84D}" name="param name" dataDxfId="108"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{1E359F77-2531-471D-845D-73EFCC64E0D2}" name="表6_8921213141516" displayName="表6_8921213141516" ref="A1:D5" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{1E359F77-2531-471D-845D-73EFCC64E0D2}" name="表6_8921213141516" displayName="表6_8921213141516" ref="A1:D5" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
   <autoFilter ref="A1:D5" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FB220119-4281-4340-9ED2-A909BBE6E90D}" name="main" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{971A8DB4-253F-4CF6-B1A5-EA9E84F48414}" name="branch" dataDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{6AC24398-79B4-4841-9B11-810FCBE7D7C3}" name="type" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{50E6A130-B526-4708-AAF2-7F8C5114E8CC}" name="param name" dataDxfId="90"/>
+    <tableColumn id="1" xr3:uid="{FB220119-4281-4340-9ED2-A909BBE6E90D}" name="main" dataDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{971A8DB4-253F-4CF6-B1A5-EA9E84F48414}" name="branch" dataDxfId="104"/>
+    <tableColumn id="3" xr3:uid="{6AC24398-79B4-4841-9B11-810FCBE7D7C3}" name="type" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{50E6A130-B526-4708-AAF2-7F8C5114E8CC}" name="param name" dataDxfId="102"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{80AE85AD-776D-48D8-A9E0-8B5B99241A3D}" name="表6_892121314151617" displayName="表6_892121314151617" ref="A1:D20" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{80AE85AD-776D-48D8-A9E0-8B5B99241A3D}" name="表6_892121314151617" displayName="表6_892121314151617" ref="A1:D20" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
   <autoFilter ref="A1:D20" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{77C5EFED-826E-40DE-9792-058A0219DB93}" name="main" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{EA04F042-A666-406F-9CE5-B964EFAFB6B1}" name="branch" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{F6F48581-298A-48A6-A7B1-5FD41B41DC85}" name="type" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{EEF330D9-79F5-4056-BECF-2EA208B917DF}" name="param name" dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{77C5EFED-826E-40DE-9792-058A0219DB93}" name="main" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{EA04F042-A666-406F-9CE5-B964EFAFB6B1}" name="branch" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{F6F48581-298A-48A6-A7B1-5FD41B41DC85}" name="type" dataDxfId="97"/>
+    <tableColumn id="4" xr3:uid="{EEF330D9-79F5-4056-BECF-2EA208B917DF}" name="param name" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{360A56DC-C9FB-415A-B518-D87DC3B610D8}" name="表6_89212131415161718" displayName="表6_89212131415161718" ref="A1:D16" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{360A56DC-C9FB-415A-B518-D87DC3B610D8}" name="表6_89212131415161718" displayName="表6_89212131415161718" ref="A1:D16" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
   <autoFilter ref="A1:D16" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{85FA0DE5-1500-4EB3-ADE2-11B529A34F3E}" name="main" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{82545C75-76EC-4363-9BE1-A1A76F81F275}" name="branch" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{96012611-D136-4234-9E88-5E00A17FA8B6}" name="type" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{7F3EEAA8-584A-41EC-A828-940B22BF5A4C}" name="param name" dataDxfId="78"/>
+    <tableColumn id="1" xr3:uid="{85FA0DE5-1500-4EB3-ADE2-11B529A34F3E}" name="main" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{82545C75-76EC-4363-9BE1-A1A76F81F275}" name="branch" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{96012611-D136-4234-9E88-5E00A17FA8B6}" name="type" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{7F3EEAA8-584A-41EC-A828-940B22BF5A4C}" name="param name" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{62FF6596-CF2A-4221-B9C6-1D41646ED98D}" name="表6_8921213141516171819" displayName="表6_8921213141516171819" ref="A1:D11" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{62FF6596-CF2A-4221-B9C6-1D41646ED98D}" name="表6_8921213141516171819" displayName="表6_8921213141516171819" ref="A1:D11" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
   <autoFilter ref="A1:D11" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5F5F8E61-AEE4-4628-9B8A-424994708189}" name="main" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{EA68617E-47E4-4E7D-A312-90D0F2B1DC4D}" name="branch" dataDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{794F68D4-D909-4EA8-962B-E2DC37B9E1B2}" name="type" dataDxfId="73"/>
-    <tableColumn id="4" xr3:uid="{BBC5FF7F-2A9F-48F7-9353-D959DA37CFB0}" name="param name" dataDxfId="72"/>
+    <tableColumn id="1" xr3:uid="{5F5F8E61-AEE4-4628-9B8A-424994708189}" name="main" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{EA68617E-47E4-4E7D-A312-90D0F2B1DC4D}" name="branch" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{794F68D4-D909-4EA8-962B-E2DC37B9E1B2}" name="type" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{BBC5FF7F-2A9F-48F7-9353-D959DA37CFB0}" name="param name" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{99C98499-87F2-4A00-A5C6-42867A84C518}" name="表6_892121314151617181920" displayName="表6_892121314151617181920" ref="A1:D32" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{99C98499-87F2-4A00-A5C6-42867A84C518}" name="表6_892121314151617181920" displayName="表6_892121314151617181920" ref="A1:D32" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
   <autoFilter ref="A1:D32" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6473C8AB-4511-4780-902D-44FF22FA9125}" name="main" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{5336CBC3-0465-44E6-842C-F8FB29DE5B60}" name="branch" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{678157D5-4DF4-42B9-BEBA-9F11FAA70230}" name="type" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{A3CD0A63-3E60-4690-8303-684CF295A686}" name="param name" dataDxfId="66"/>
+    <tableColumn id="1" xr3:uid="{6473C8AB-4511-4780-902D-44FF22FA9125}" name="main" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{5336CBC3-0465-44E6-842C-F8FB29DE5B60}" name="branch" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{678157D5-4DF4-42B9-BEBA-9F11FAA70230}" name="type" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{A3CD0A63-3E60-4690-8303-684CF295A686}" name="param name" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EBE48E62-3111-4EF7-9659-DEC591C84F2E}" name="表3" displayName="表3" ref="A1:D22" totalsRowShown="0" headerRowDxfId="178" dataDxfId="176" headerRowBorderDxfId="177" tableBorderDxfId="175" totalsRowBorderDxfId="174">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EBE48E62-3111-4EF7-9659-DEC591C84F2E}" name="表3" displayName="表3" ref="A1:D22" totalsRowShown="0" headerRowDxfId="190" dataDxfId="188" headerRowBorderDxfId="189" tableBorderDxfId="187" totalsRowBorderDxfId="186">
   <autoFilter ref="A1:D22" xr:uid="{EBE48E62-3111-4EF7-9659-DEC591C84F2E}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A9C5E782-2908-495B-BC1E-48E2FD18AEE0}" name="main" dataDxfId="173"/>
-    <tableColumn id="2" xr3:uid="{5470BF63-58F6-4E58-9D4F-C002B557215E}" name="branch" dataDxfId="172"/>
-    <tableColumn id="3" xr3:uid="{90636DC2-3EDA-473A-801B-DF14180D5E8D}" name="type" dataDxfId="171"/>
-    <tableColumn id="4" xr3:uid="{73405289-D597-4AE2-A24C-A23D026B4D06}" name="param name" dataDxfId="170"/>
+    <tableColumn id="1" xr3:uid="{A9C5E782-2908-495B-BC1E-48E2FD18AEE0}" name="main" dataDxfId="185"/>
+    <tableColumn id="2" xr3:uid="{5470BF63-58F6-4E58-9D4F-C002B557215E}" name="branch" dataDxfId="184"/>
+    <tableColumn id="3" xr3:uid="{90636DC2-3EDA-473A-801B-DF14180D5E8D}" name="type" dataDxfId="183"/>
+    <tableColumn id="4" xr3:uid="{73405289-D597-4AE2-A24C-A23D026B4D06}" name="param name" dataDxfId="182"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{B9092D73-1E82-43D3-BB36-1B82F1AB4C19}" name="表6_89212131415161718192021" displayName="表6_89212131415161718192021" ref="A1:D4" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{B9092D73-1E82-43D3-BB36-1B82F1AB4C19}" name="表6_89212131415161718192021" displayName="表6_89212131415161718192021" ref="A1:D4" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
   <autoFilter ref="A1:D4" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{446C90BC-EE13-48AF-8953-B0823F1EF424}" name="main" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{A4BE9E1C-DCDF-4035-B22F-975533B7EE8E}" name="branch" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{F066C877-271A-431C-9942-DB3171BA218A}" name="type" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{4DCDA06A-8121-4C10-882B-A92225C0E935}" name="param name" dataDxfId="60"/>
+    <tableColumn id="1" xr3:uid="{446C90BC-EE13-48AF-8953-B0823F1EF424}" name="main" dataDxfId="75"/>
+    <tableColumn id="2" xr3:uid="{A4BE9E1C-DCDF-4035-B22F-975533B7EE8E}" name="branch" dataDxfId="74"/>
+    <tableColumn id="3" xr3:uid="{F066C877-271A-431C-9942-DB3171BA218A}" name="type" dataDxfId="73"/>
+    <tableColumn id="4" xr3:uid="{4DCDA06A-8121-4C10-882B-A92225C0E935}" name="param name" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{A6640308-7007-4510-842B-DAAD60ED3552}" name="表6_8921213141516171819202122" displayName="表6_8921213141516171819202122" ref="A1:D7" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{A6640308-7007-4510-842B-DAAD60ED3552}" name="表6_8921213141516171819202122" displayName="表6_8921213141516171819202122" ref="A1:D7" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
   <autoFilter ref="A1:D7" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BE0266B4-0AA2-475C-8D13-DBDF17FE05C3}" name="main" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{E7D086AD-F1E1-47EE-A908-729CC7D1EDB9}" name="branch" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{30879BC5-4F3C-4CE6-81C1-426176CBF96F}" name="type" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{C2372A9E-8322-4203-8AD8-9EF37FB73D2B}" name="param name" dataDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{BE0266B4-0AA2-475C-8D13-DBDF17FE05C3}" name="main" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{E7D086AD-F1E1-47EE-A908-729CC7D1EDB9}" name="branch" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{30879BC5-4F3C-4CE6-81C1-426176CBF96F}" name="type" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{C2372A9E-8322-4203-8AD8-9EF37FB73D2B}" name="param name" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{844A6BA8-C36D-413A-B54D-E7B75700C5B0}" name="表6_892121314151617181920212223" displayName="表6_892121314151617181920212223" ref="A1:D12" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{844A6BA8-C36D-413A-B54D-E7B75700C5B0}" name="表6_892121314151617181920212223" displayName="表6_892121314151617181920212223" ref="A1:D12" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
   <autoFilter ref="A1:D12" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{EA39BB2F-8FC6-4310-8EB3-E2D37B6D1DE6}" name="main" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{E957548F-271C-40B2-9092-CE9C0E9F6144}" name="branch" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{9382DDB7-EB44-4420-A985-2B29EB05A1AB}" name="type" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{92812206-9544-4249-A90A-3C34475D1723}" name="param name" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{EA39BB2F-8FC6-4310-8EB3-E2D37B6D1DE6}" name="main" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{E957548F-271C-40B2-9092-CE9C0E9F6144}" name="branch" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{9382DDB7-EB44-4420-A985-2B29EB05A1AB}" name="type" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{92812206-9544-4249-A90A-3C34475D1723}" name="param name" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{2AF21F10-51C5-4833-A199-42225D1D6730}" name="表6_89212131415161718192021222324" displayName="表6_89212131415161718192021222324" ref="A1:D228" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{2AF21F10-51C5-4833-A199-42225D1D6730}" name="表6_89212131415161718192021222324" displayName="表6_89212131415161718192021222324" ref="A1:D228" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="A1:D228" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}">
     <filterColumn colId="3">
       <filters>
@@ -5007,17 +5100,17 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{1CEEBD0F-DE94-484C-8FDC-176AF6899DE4}" name="main" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{4748AC76-F26C-4A8E-B7FD-51E3A961A0DB}" name="branch" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{EE6CB704-AFEC-4814-B724-8C974D2C1C4A}" name="type" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{21049C3B-A088-4554-A135-9BFC4E507614}" name="param name" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{1CEEBD0F-DE94-484C-8FDC-176AF6899DE4}" name="main" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{4748AC76-F26C-4A8E-B7FD-51E3A961A0DB}" name="branch" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{EE6CB704-AFEC-4814-B724-8C974D2C1C4A}" name="type" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{21049C3B-A088-4554-A135-9BFC4E507614}" name="param name" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{55BF17C4-35F9-443B-B504-6F8CF153E765}" name="表6_8921213141516171819202122232425" displayName="表6_8921213141516171819202122232425" ref="A1:D128" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{55BF17C4-35F9-443B-B504-6F8CF153E765}" name="表6_8921213141516171819202122232425" displayName="表6_8921213141516171819202122232425" ref="A1:D128" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="A1:D128" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}">
     <filterColumn colId="3">
       <filters>
@@ -5033,17 +5126,17 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{67C559A2-2EC4-4EA5-AC44-6F0B83853E07}" name="main" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{5062C9AC-3913-48C1-AACB-3DC177626C6D}" name="branch" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{8D2188A2-6728-48FB-81FE-331F3F410AEA}" name="type" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{7FAF264C-841C-41C7-8F4F-56EDB6D7C8B3}" name="param name" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{67C559A2-2EC4-4EA5-AC44-6F0B83853E07}" name="main" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{5062C9AC-3913-48C1-AACB-3DC177626C6D}" name="branch" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{8D2188A2-6728-48FB-81FE-331F3F410AEA}" name="type" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{7FAF264C-841C-41C7-8F4F-56EDB6D7C8B3}" name="param name" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{8D619451-02A5-419F-AD3C-FE8AECE06AD8}" name="表6_892121314151617181920212223242526" displayName="表6_892121314151617181920212223242526" ref="A1:D148" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{8D619451-02A5-419F-AD3C-FE8AECE06AD8}" name="表6_892121314151617181920212223242526" displayName="表6_892121314151617181920212223242526" ref="A1:D148" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="A1:D148" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}">
     <filterColumn colId="3">
       <filters>
@@ -5054,166 +5147,203 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9D656239-4345-464E-9E4D-F546800A4D9E}" name="main" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{A403BB16-00B7-4984-91F8-80C98BEDFAE9}" name="branch" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{18F2EC94-873F-4403-9B63-44BA4485862E}" name="type" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{4BF4EB5D-4276-4036-94F4-BD977DD08A32}" name="param name" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{9D656239-4345-464E-9E4D-F546800A4D9E}" name="main" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{A403BB16-00B7-4984-91F8-80C98BEDFAE9}" name="branch" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{18F2EC94-873F-4403-9B63-44BA4485862E}" name="type" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{4BF4EB5D-4276-4036-94F4-BD977DD08A32}" name="param name" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{D77823DB-C201-4E7D-833C-6085CF94DD96}" name="表6_89212131415161718192021222324252627" displayName="表6_89212131415161718192021222324252627" ref="A1:D18" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{D77823DB-C201-4E7D-833C-6085CF94DD96}" name="表6_89212131415161718192021222324252627" displayName="表6_89212131415161718192021222324252627" ref="A1:D18" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="A1:D18" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C99D0936-A00D-473A-9722-7AB9594E93FA}" name="main" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{91ED2A21-20F7-4D7F-8995-D255AD21FD6C}" name="branch" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{704694F5-EE15-4077-A55A-68AB0FC0A262}" name="type" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{EB568756-ADFD-452D-9F00-E142C274E911}" name="param name" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{C99D0936-A00D-473A-9722-7AB9594E93FA}" name="main" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{91ED2A21-20F7-4D7F-8995-D255AD21FD6C}" name="branch" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{704694F5-EE15-4077-A55A-68AB0FC0A262}" name="type" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{EB568756-ADFD-452D-9F00-E142C274E911}" name="param name" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{120987A5-0656-40F2-B4C8-58BDD36818AF}" name="表6_8921213141516171819202122232425262728" displayName="表6_8921213141516171819202122232425262728" ref="A1:D25" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{120987A5-0656-40F2-B4C8-58BDD36818AF}" name="表6_8921213141516171819202122232425262728" displayName="表6_8921213141516171819202122232425262728" ref="A1:D25" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A1:D25" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D3F0BF9B-EF3D-46FD-851B-DE7A8BA6861A}" name="main" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{26734EFB-3A91-4358-8F49-76CD28502CCD}" name="branch" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{21B8E7A3-96A6-4FA8-BF69-2D45AD6CE016}" name="type" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{DFD55D6B-2A70-453A-A9CA-3AC307D52CEB}" name="param name" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{D3F0BF9B-EF3D-46FD-851B-DE7A8BA6861A}" name="main" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{26734EFB-3A91-4358-8F49-76CD28502CCD}" name="branch" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{21B8E7A3-96A6-4FA8-BF69-2D45AD6CE016}" name="type" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{DFD55D6B-2A70-453A-A9CA-3AC307D52CEB}" name="param name" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{9E1029A9-E2B6-460A-BDD3-35B9E8EF1A27}" name="表6_892121314151617181920212223242526272829" displayName="表6_892121314151617181920212223242526272829" ref="A1:D37" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{9E1029A9-E2B6-460A-BDD3-35B9E8EF1A27}" name="表6_892121314151617181920212223242526272829" displayName="表6_892121314151617181920212223242526272829" ref="A1:D37" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A1:D37" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{202FE0DE-0C42-49BE-8A93-547C5E684986}" name="main" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{1D731C2C-7DC2-450C-A501-23252C619AFE}" name="branch" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{F7069DC3-74B6-41AD-BA7F-D8AD59F0EFD6}" name="type" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{5A9F1D1F-D443-4878-97A8-CA433BC066DD}" name="param name" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{202FE0DE-0C42-49BE-8A93-547C5E684986}" name="main" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{1D731C2C-7DC2-450C-A501-23252C619AFE}" name="branch" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{F7069DC3-74B6-41AD-BA7F-D8AD59F0EFD6}" name="type" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{5A9F1D1F-D443-4878-97A8-CA433BC066DD}" name="param name" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{812EF589-76F5-45DE-814A-25389EF0967B}" name="表6_89212131415161718192021222324252627282930" displayName="表6_89212131415161718192021222324252627282930" ref="A1:D86" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:D86" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{812EF589-76F5-45DE-814A-25389EF0967B}" name="表6_89212131415161718192021222324252627282930" displayName="表6_89212131415161718192021222324252627282930" ref="A1:D86" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:D86" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="texmap_base_bump"/>
+        <filter val="texmap_base_bump_multiplier"/>
+        <filter val="texmap_base_bump_on"/>
+        <filter val="texmap_coat_bump"/>
+        <filter val="texmap_coat_bump_multiplier"/>
+        <filter val="texmap_coat_bump_on"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8F1AA2F5-9662-4F90-9B63-332419C63823}" name="main" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{42B506CD-7BCF-42F9-BC3C-1D006F57004F}" name="branch" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{317A53D1-91A1-461D-8658-2B7B138E7753}" name="type" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{D5F70997-D51C-452C-89F1-F64CC91C8011}" name="param name" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{8F1AA2F5-9662-4F90-9B63-332419C63823}" name="main" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{42B506CD-7BCF-42F9-BC3C-1D006F57004F}" name="branch" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{317A53D1-91A1-461D-8658-2B7B138E7753}" name="type" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{D5F70997-D51C-452C-89F1-F64CC91C8011}" name="param name" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{394FAB82-2B71-4FB2-B8AF-E823A9D706D4}" name="表4" displayName="表4" ref="A1:D14" totalsRowShown="0" headerRowDxfId="169" dataDxfId="168">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{394FAB82-2B71-4FB2-B8AF-E823A9D706D4}" name="表4" displayName="表4" ref="A1:D14" totalsRowShown="0" headerRowDxfId="181" dataDxfId="180">
   <autoFilter ref="A1:D14" xr:uid="{394FAB82-2B71-4FB2-B8AF-E823A9D706D4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3808606C-1404-4259-B39E-E1E7A110B5CA}" name="main" dataDxfId="167"/>
-    <tableColumn id="2" xr3:uid="{F328710A-D3E3-4CE0-96F6-91F65F558FA0}" name="branch" dataDxfId="166"/>
-    <tableColumn id="3" xr3:uid="{DFCF2074-8826-4ED3-870D-7F464F5BEA44}" name="type" dataDxfId="165"/>
-    <tableColumn id="4" xr3:uid="{229BF5C0-6908-4BBD-A508-EF45263F6BC0}" name="param name" dataDxfId="164"/>
+    <tableColumn id="1" xr3:uid="{3808606C-1404-4259-B39E-E1E7A110B5CA}" name="main" dataDxfId="179"/>
+    <tableColumn id="2" xr3:uid="{F328710A-D3E3-4CE0-96F6-91F65F558FA0}" name="branch" dataDxfId="178"/>
+    <tableColumn id="3" xr3:uid="{DFCF2074-8826-4ED3-870D-7F464F5BEA44}" name="type" dataDxfId="177"/>
+    <tableColumn id="4" xr3:uid="{229BF5C0-6908-4BBD-A508-EF45263F6BC0}" name="param name" dataDxfId="176"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{1D60048A-C472-4872-AC9D-2379248F9D6F}" name="表6_8921213141516171819202122232425262728293031" displayName="表6_8921213141516171819202122232425262728293031" ref="A1:D2" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{1D60048A-C472-4872-AC9D-2379248F9D6F}" name="表6_8921213141516171819202122232425262728293031" displayName="表6_8921213141516171819202122232425262728293031" ref="A1:D2" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A1:D2" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D7A2469D-F5D2-40F7-BAB6-BA297295D345}" name="main" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{6877823A-086B-468B-83BF-BB42DD98E006}" name="branch" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{37B4F256-51D2-421F-B0A5-2CBFDC7ABAA8}" name="type" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{9AC80006-A126-46BA-9F52-749AB1F7286A}" name="param name" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D7A2469D-F5D2-40F7-BAB6-BA297295D345}" name="main" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{6877823A-086B-468B-83BF-BB42DD98E006}" name="branch" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{37B4F256-51D2-421F-B0A5-2CBFDC7ABAA8}" name="type" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{9AC80006-A126-46BA-9F52-749AB1F7286A}" name="param name" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{42393325-2B83-4B11-82F6-EFBF38BDEDFC}" name="表6_892121314151617181920212223242526272829303132" displayName="表6_892121314151617181920212223242526272829303132" ref="A1:D2" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:D2" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{F0DA75C7-FB66-46BD-A5A7-A150C0AAA29F}" name="main" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{335B8FD7-F4F5-4C0C-A754-A72950A1BE9B}" name="branch" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{E662F644-60D2-4DC7-90DE-A01BB09AF019}" name="type" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{8D1177B3-DA60-4E28-96E4-F084155D116A}" name="param name" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{386C923B-D958-43D1-B3BB-6151D778DC29}" name="表6_89212131415161718192021222324252627282930313233" displayName="表6_89212131415161718192021222324252627282930313233" ref="A1:D2" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D2" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{D55E2339-875B-4D76-A3FA-D3B13080AEA4}" name="main" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{E91F64E1-4386-462F-B3A8-EE83BD90C51B}" name="branch" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{3271998A-703F-4CF6-9450-42971CBBB68B}" name="type" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{6E633AD3-7444-46B0-8CD2-C71AF9825721}" name="param name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AAA7849C-C24E-440E-83A7-D46AEB062254}" name="表5" displayName="表5" ref="A1:D36" totalsRowShown="0" headerRowDxfId="163" headerRowBorderDxfId="162" tableBorderDxfId="161" totalsRowBorderDxfId="160">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AAA7849C-C24E-440E-83A7-D46AEB062254}" name="表5" displayName="表5" ref="A1:D36" totalsRowShown="0" headerRowDxfId="175" headerRowBorderDxfId="174" tableBorderDxfId="173" totalsRowBorderDxfId="172">
   <autoFilter ref="A1:D36" xr:uid="{AAA7849C-C24E-440E-83A7-D46AEB062254}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4AE65613-9E32-4B81-B096-3CE2F9469A99}" name="main" dataDxfId="159"/>
-    <tableColumn id="2" xr3:uid="{B9C8132D-EB95-4F97-B376-375C1E78DA2F}" name="branch" dataDxfId="158"/>
-    <tableColumn id="3" xr3:uid="{A1B42A52-7EC8-4E70-A45E-3F416909E1EA}" name="type" dataDxfId="157"/>
-    <tableColumn id="4" xr3:uid="{390F265C-3120-4E30-9A3E-68BE2347C969}" name="param name" dataDxfId="156"/>
+    <tableColumn id="1" xr3:uid="{4AE65613-9E32-4B81-B096-3CE2F9469A99}" name="main" dataDxfId="171"/>
+    <tableColumn id="2" xr3:uid="{B9C8132D-EB95-4F97-B376-375C1E78DA2F}" name="branch" dataDxfId="170"/>
+    <tableColumn id="3" xr3:uid="{A1B42A52-7EC8-4E70-A45E-3F416909E1EA}" name="type" dataDxfId="169"/>
+    <tableColumn id="4" xr3:uid="{390F265C-3120-4E30-9A3E-68BE2347C969}" name="param name" dataDxfId="168"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}" name="表6" displayName="表6" ref="A1:D17" totalsRowShown="0" headerRowDxfId="155" dataDxfId="154">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}" name="表6" displayName="表6" ref="A1:D17" totalsRowShown="0" headerRowDxfId="167" dataDxfId="166">
   <autoFilter ref="A1:D17" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BAEEF277-80BF-4C16-8215-7CCD39C11565}" name="main" dataDxfId="153"/>
-    <tableColumn id="2" xr3:uid="{45843013-F77E-4A90-AF54-173129A318BC}" name="branch" dataDxfId="152"/>
-    <tableColumn id="3" xr3:uid="{DE07E8D7-AF19-4990-B4EB-FB8A48054E6D}" name="type" dataDxfId="151"/>
-    <tableColumn id="4" xr3:uid="{D87A2779-3B12-41B3-968D-150307DF3484}" name="param name" dataDxfId="150"/>
+    <tableColumn id="1" xr3:uid="{BAEEF277-80BF-4C16-8215-7CCD39C11565}" name="main" dataDxfId="165"/>
+    <tableColumn id="2" xr3:uid="{45843013-F77E-4A90-AF54-173129A318BC}" name="branch" dataDxfId="164"/>
+    <tableColumn id="3" xr3:uid="{DE07E8D7-AF19-4990-B4EB-FB8A48054E6D}" name="type" dataDxfId="163"/>
+    <tableColumn id="4" xr3:uid="{D87A2779-3B12-41B3-968D-150307DF3484}" name="param name" dataDxfId="162"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44179487-8091-4992-8094-4DA31A4A9A12}" name="表6_8" displayName="表6_8" ref="A1:D8" totalsRowShown="0" headerRowDxfId="149" dataDxfId="148">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44179487-8091-4992-8094-4DA31A4A9A12}" name="表6_8" displayName="表6_8" ref="A1:D8" totalsRowShown="0" headerRowDxfId="161" dataDxfId="160">
   <autoFilter ref="A1:D8" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{74AA3551-D5FC-442E-820B-56B35F04E314}" name="main" dataDxfId="147"/>
-    <tableColumn id="2" xr3:uid="{872A74B1-DD5D-4A36-ADFF-F85B7DA48580}" name="branch" dataDxfId="146"/>
-    <tableColumn id="3" xr3:uid="{92E7DF35-9ECD-40C3-9E4D-BD067B6A62EC}" name="type" dataDxfId="145"/>
-    <tableColumn id="4" xr3:uid="{521BB435-4AEA-479B-9B1C-8DE67307817F}" name="param name" dataDxfId="144"/>
+    <tableColumn id="1" xr3:uid="{74AA3551-D5FC-442E-820B-56B35F04E314}" name="main" dataDxfId="159"/>
+    <tableColumn id="2" xr3:uid="{872A74B1-DD5D-4A36-ADFF-F85B7DA48580}" name="branch" dataDxfId="158"/>
+    <tableColumn id="3" xr3:uid="{92E7DF35-9ECD-40C3-9E4D-BD067B6A62EC}" name="type" dataDxfId="157"/>
+    <tableColumn id="4" xr3:uid="{521BB435-4AEA-479B-9B1C-8DE67307817F}" name="param name" dataDxfId="156"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{C4239BEF-66B1-4C30-A627-2C7A8F2E4BA9}" name="表6_89" displayName="表6_89" ref="A1:D7" totalsRowShown="0" headerRowDxfId="143" dataDxfId="142">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{C4239BEF-66B1-4C30-A627-2C7A8F2E4BA9}" name="表6_89" displayName="表6_89" ref="A1:D7" totalsRowShown="0" headerRowDxfId="155" dataDxfId="154">
   <autoFilter ref="A1:D7" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8A8D086D-6A95-4C02-8C03-468264AB5725}" name="main" dataDxfId="141"/>
-    <tableColumn id="2" xr3:uid="{CE92D93E-D841-4961-B94A-11AA4C235B48}" name="branch" dataDxfId="140"/>
-    <tableColumn id="3" xr3:uid="{9EA0702F-1E71-4F31-A149-4EDC82F3059F}" name="type" dataDxfId="139"/>
-    <tableColumn id="4" xr3:uid="{1126922B-B081-42BE-9F6D-8F699D3E6FEF}" name="param name" dataDxfId="138"/>
+    <tableColumn id="1" xr3:uid="{8A8D086D-6A95-4C02-8C03-468264AB5725}" name="main" dataDxfId="153"/>
+    <tableColumn id="2" xr3:uid="{CE92D93E-D841-4961-B94A-11AA4C235B48}" name="branch" dataDxfId="152"/>
+    <tableColumn id="3" xr3:uid="{9EA0702F-1E71-4F31-A149-4EDC82F3059F}" name="type" dataDxfId="151"/>
+    <tableColumn id="4" xr3:uid="{1126922B-B081-42BE-9F6D-8F699D3E6FEF}" name="param name" dataDxfId="150"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{2F70E97C-7386-4083-8729-2F25C3160A9B}" name="表6_8910" displayName="表6_8910" ref="A1:D22" totalsRowShown="0" headerRowDxfId="137" dataDxfId="136">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{2F70E97C-7386-4083-8729-2F25C3160A9B}" name="表6_8910" displayName="表6_8910" ref="A1:D22" totalsRowShown="0" headerRowDxfId="149" dataDxfId="148">
   <autoFilter ref="A1:D22" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0177998A-43AB-4B0F-8604-0AF954FBB185}" name="main" dataDxfId="135"/>
-    <tableColumn id="2" xr3:uid="{37520786-1F3E-4E38-8C3B-6E990C026213}" name="branch" dataDxfId="134"/>
-    <tableColumn id="3" xr3:uid="{06224467-73DA-4D97-B072-2FA1C3A7CF43}" name="type" dataDxfId="133"/>
-    <tableColumn id="4" xr3:uid="{7F4CE11F-D886-48B2-A97A-A561D4C6C79B}" name="param name" dataDxfId="132"/>
+    <tableColumn id="1" xr3:uid="{0177998A-43AB-4B0F-8604-0AF954FBB185}" name="main" dataDxfId="147"/>
+    <tableColumn id="2" xr3:uid="{37520786-1F3E-4E38-8C3B-6E990C026213}" name="branch" dataDxfId="146"/>
+    <tableColumn id="3" xr3:uid="{06224467-73DA-4D97-B072-2FA1C3A7CF43}" name="type" dataDxfId="145"/>
+    <tableColumn id="4" xr3:uid="{7F4CE11F-D886-48B2-A97A-A561D4C6C79B}" name="param name" dataDxfId="144"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{F6E123A4-AC18-4383-8FEF-88FC9710A391}" name="表6_891011" displayName="表6_891011" ref="A1:D48" totalsRowShown="0" headerRowDxfId="131" dataDxfId="130">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{F6E123A4-AC18-4383-8FEF-88FC9710A391}" name="表6_891011" displayName="表6_891011" ref="A1:D48" totalsRowShown="0" headerRowDxfId="143" dataDxfId="142">
   <autoFilter ref="A1:D48" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8A85C0EA-4CDE-4D93-B049-3C11FD83B866}" name="main" dataDxfId="129"/>
-    <tableColumn id="2" xr3:uid="{B4D689B8-7678-4627-8C30-571AFA1954CE}" name="branch" dataDxfId="128"/>
-    <tableColumn id="3" xr3:uid="{1B0A04CF-F3AC-4373-A92B-F7D319E52FC4}" name="type" dataDxfId="127"/>
-    <tableColumn id="4" xr3:uid="{5B52C9B4-0914-412B-8D7D-C4F1D3CB6CA9}" name="param name" dataDxfId="126"/>
+    <tableColumn id="1" xr3:uid="{8A85C0EA-4CDE-4D93-B049-3C11FD83B866}" name="main" dataDxfId="141"/>
+    <tableColumn id="2" xr3:uid="{B4D689B8-7678-4627-8C30-571AFA1954CE}" name="branch" dataDxfId="140"/>
+    <tableColumn id="3" xr3:uid="{1B0A04CF-F3AC-4373-A92B-F7D319E52FC4}" name="type" dataDxfId="139"/>
+    <tableColumn id="4" xr3:uid="{5B52C9B4-0914-412B-8D7D-C4F1D3CB6CA9}" name="param name" dataDxfId="138"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -16184,7 +16314,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D18"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -16460,8 +16590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C36C744-F1C4-49B8-ABE3-C3460864E11C}">
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -17540,8 +17670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8752D82F-8718-46C8-BE35-DD85418B6463}">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -17566,7 +17696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14">
         <v>0</v>
       </c>
@@ -17580,11 +17710,11 @@
         <v>838</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="19">
-        <v>0</v>
-      </c>
-      <c r="B3" s="19">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14">
         <v>1</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -17594,11 +17724,11 @@
         <v>839</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="19">
-        <v>0</v>
-      </c>
-      <c r="B4" s="19">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="14">
+        <v>0</v>
+      </c>
+      <c r="B4" s="14">
         <v>2</v>
       </c>
       <c r="C4" s="15" t="s">
@@ -17608,11 +17738,11 @@
         <v>840</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="19">
-        <v>0</v>
-      </c>
-      <c r="B5" s="19">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="14">
+        <v>0</v>
+      </c>
+      <c r="B5" s="14">
         <v>3</v>
       </c>
       <c r="C5" s="15" t="s">
@@ -17622,11 +17752,11 @@
         <v>841</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="19">
-        <v>0</v>
-      </c>
-      <c r="B6" s="19">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="14">
+        <v>0</v>
+      </c>
+      <c r="B6" s="14">
         <v>4</v>
       </c>
       <c r="C6" s="15" t="s">
@@ -17636,11 +17766,11 @@
         <v>842</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="19">
-        <v>0</v>
-      </c>
-      <c r="B7" s="19">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="14">
+        <v>0</v>
+      </c>
+      <c r="B7" s="14">
         <v>5</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -17650,11 +17780,11 @@
         <v>843</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="19">
-        <v>0</v>
-      </c>
-      <c r="B8" s="19">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="14">
+        <v>0</v>
+      </c>
+      <c r="B8" s="14">
         <v>6</v>
       </c>
       <c r="C8" s="15" t="s">
@@ -17664,11 +17794,11 @@
         <v>844</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="19">
-        <v>0</v>
-      </c>
-      <c r="B9" s="19">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="14">
+        <v>0</v>
+      </c>
+      <c r="B9" s="14">
         <v>7</v>
       </c>
       <c r="C9" s="15" t="s">
@@ -17678,11 +17808,11 @@
         <v>845</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="19">
-        <v>0</v>
-      </c>
-      <c r="B10" s="19">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="14">
+        <v>0</v>
+      </c>
+      <c r="B10" s="14">
         <v>8</v>
       </c>
       <c r="C10" s="15" t="s">
@@ -17692,11 +17822,11 @@
         <v>846</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="19">
-        <v>0</v>
-      </c>
-      <c r="B11" s="19">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="14">
+        <v>0</v>
+      </c>
+      <c r="B11" s="14">
         <v>9</v>
       </c>
       <c r="C11" s="15" t="s">
@@ -17706,11 +17836,11 @@
         <v>847</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="19">
-        <v>0</v>
-      </c>
-      <c r="B12" s="19">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="14">
+        <v>0</v>
+      </c>
+      <c r="B12" s="14">
         <v>10</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -17720,11 +17850,11 @@
         <v>848</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="19">
-        <v>0</v>
-      </c>
-      <c r="B13" s="19">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="14">
+        <v>0</v>
+      </c>
+      <c r="B13" s="14">
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
@@ -17734,11 +17864,11 @@
         <v>849</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="19">
-        <v>0</v>
-      </c>
-      <c r="B14" s="19">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="14">
+        <v>0</v>
+      </c>
+      <c r="B14" s="14">
         <v>12</v>
       </c>
       <c r="C14" s="15" t="s">
@@ -17748,11 +17878,11 @@
         <v>850</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="19">
-        <v>0</v>
-      </c>
-      <c r="B15" s="19">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="14">
+        <v>0</v>
+      </c>
+      <c r="B15" s="14">
         <v>13</v>
       </c>
       <c r="C15" s="15" t="s">
@@ -17762,11 +17892,11 @@
         <v>851</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="19">
-        <v>0</v>
-      </c>
-      <c r="B16" s="19">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="14">
+        <v>0</v>
+      </c>
+      <c r="B16" s="14">
         <v>14</v>
       </c>
       <c r="C16" s="15" t="s">
@@ -17776,11 +17906,11 @@
         <v>852</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="19">
-        <v>0</v>
-      </c>
-      <c r="B17" s="19">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="14">
+        <v>0</v>
+      </c>
+      <c r="B17" s="14">
         <v>15</v>
       </c>
       <c r="C17" s="15" t="s">
@@ -17790,11 +17920,11 @@
         <v>853</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="19">
-        <v>0</v>
-      </c>
-      <c r="B18" s="19">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="14">
+        <v>0</v>
+      </c>
+      <c r="B18" s="14">
         <v>16</v>
       </c>
       <c r="C18" s="15" t="s">
@@ -17804,11 +17934,11 @@
         <v>854</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="19">
-        <v>0</v>
-      </c>
-      <c r="B19" s="19">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="14">
+        <v>0</v>
+      </c>
+      <c r="B19" s="14">
         <v>17</v>
       </c>
       <c r="C19" s="15" t="s">
@@ -17818,11 +17948,11 @@
         <v>855</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="19">
-        <v>0</v>
-      </c>
-      <c r="B20" s="19">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="14">
+        <v>0</v>
+      </c>
+      <c r="B20" s="14">
         <v>18</v>
       </c>
       <c r="C20" s="15" t="s">
@@ -17832,11 +17962,11 @@
         <v>856</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="19">
-        <v>0</v>
-      </c>
-      <c r="B21" s="19">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="14">
+        <v>0</v>
+      </c>
+      <c r="B21" s="14">
         <v>19</v>
       </c>
       <c r="C21" s="15" t="s">
@@ -17846,11 +17976,11 @@
         <v>857</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="19">
-        <v>0</v>
-      </c>
-      <c r="B22" s="19">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="14">
+        <v>0</v>
+      </c>
+      <c r="B22" s="14">
         <v>20</v>
       </c>
       <c r="C22" s="15" t="s">
@@ -17860,11 +17990,11 @@
         <v>858</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="19">
-        <v>0</v>
-      </c>
-      <c r="B23" s="19">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="14">
+        <v>0</v>
+      </c>
+      <c r="B23" s="14">
         <v>21</v>
       </c>
       <c r="C23" s="15" t="s">
@@ -17874,11 +18004,11 @@
         <v>859</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="19">
-        <v>0</v>
-      </c>
-      <c r="B24" s="19">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="14">
+        <v>0</v>
+      </c>
+      <c r="B24" s="14">
         <v>22</v>
       </c>
       <c r="C24" s="15" t="s">
@@ -17888,11 +18018,11 @@
         <v>860</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="19">
-        <v>0</v>
-      </c>
-      <c r="B25" s="19">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="14">
+        <v>0</v>
+      </c>
+      <c r="B25" s="14">
         <v>23</v>
       </c>
       <c r="C25" s="15" t="s">
@@ -17902,11 +18032,11 @@
         <v>861</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="19">
-        <v>0</v>
-      </c>
-      <c r="B26" s="19">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="14">
+        <v>0</v>
+      </c>
+      <c r="B26" s="14">
         <v>24</v>
       </c>
       <c r="C26" s="15" t="s">
@@ -17916,11 +18046,11 @@
         <v>862</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="19">
-        <v>0</v>
-      </c>
-      <c r="B27" s="19">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="14">
+        <v>0</v>
+      </c>
+      <c r="B27" s="14">
         <v>25</v>
       </c>
       <c r="C27" s="15" t="s">
@@ -17930,11 +18060,11 @@
         <v>863</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="19">
-        <v>0</v>
-      </c>
-      <c r="B28" s="19">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="14">
+        <v>0</v>
+      </c>
+      <c r="B28" s="14">
         <v>26</v>
       </c>
       <c r="C28" s="15" t="s">
@@ -17944,11 +18074,11 @@
         <v>393</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="19">
-        <v>0</v>
-      </c>
-      <c r="B29" s="19">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="14">
+        <v>0</v>
+      </c>
+      <c r="B29" s="14">
         <v>27</v>
       </c>
       <c r="C29" s="15" t="s">
@@ -17958,11 +18088,11 @@
         <v>864</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="19">
-        <v>0</v>
-      </c>
-      <c r="B30" s="19">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="14">
+        <v>0</v>
+      </c>
+      <c r="B30" s="14">
         <v>28</v>
       </c>
       <c r="C30" s="15" t="s">
@@ -17972,11 +18102,11 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="19">
-        <v>0</v>
-      </c>
-      <c r="B31" s="19">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="14">
+        <v>0</v>
+      </c>
+      <c r="B31" s="14">
         <v>29</v>
       </c>
       <c r="C31" s="15" t="s">
@@ -17986,11 +18116,11 @@
         <v>865</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="19">
-        <v>0</v>
-      </c>
-      <c r="B32" s="19">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="14">
+        <v>0</v>
+      </c>
+      <c r="B32" s="14">
         <v>30</v>
       </c>
       <c r="C32" s="15" t="s">
@@ -18000,11 +18130,11 @@
         <v>396</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="19">
-        <v>0</v>
-      </c>
-      <c r="B33" s="19">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="14">
+        <v>0</v>
+      </c>
+      <c r="B33" s="14">
         <v>31</v>
       </c>
       <c r="C33" s="15" t="s">
@@ -18014,11 +18144,11 @@
         <v>866</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="19">
-        <v>0</v>
-      </c>
-      <c r="B34" s="19">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="14">
+        <v>0</v>
+      </c>
+      <c r="B34" s="14">
         <v>32</v>
       </c>
       <c r="C34" s="15" t="s">
@@ -18028,11 +18158,11 @@
         <v>395</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="19">
-        <v>0</v>
-      </c>
-      <c r="B35" s="19">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="14">
+        <v>0</v>
+      </c>
+      <c r="B35" s="14">
         <v>33</v>
       </c>
       <c r="C35" s="15" t="s">
@@ -18042,11 +18172,11 @@
         <v>867</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="19">
-        <v>0</v>
-      </c>
-      <c r="B36" s="19">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="14">
+        <v>0</v>
+      </c>
+      <c r="B36" s="14">
         <v>34</v>
       </c>
       <c r="C36" s="15" t="s">
@@ -18056,11 +18186,11 @@
         <v>868</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="19">
-        <v>0</v>
-      </c>
-      <c r="B37" s="19">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="14">
+        <v>0</v>
+      </c>
+      <c r="B37" s="14">
         <v>35</v>
       </c>
       <c r="C37" s="15" t="s">
@@ -18070,11 +18200,11 @@
         <v>869</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="19">
-        <v>0</v>
-      </c>
-      <c r="B38" s="19">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="14">
+        <v>0</v>
+      </c>
+      <c r="B38" s="14">
         <v>36</v>
       </c>
       <c r="C38" s="15" t="s">
@@ -18084,11 +18214,11 @@
         <v>870</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="19">
-        <v>0</v>
-      </c>
-      <c r="B39" s="19">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="14">
+        <v>0</v>
+      </c>
+      <c r="B39" s="14">
         <v>37</v>
       </c>
       <c r="C39" s="15" t="s">
@@ -18098,11 +18228,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="19">
-        <v>0</v>
-      </c>
-      <c r="B40" s="19">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="14">
+        <v>0</v>
+      </c>
+      <c r="B40" s="14">
         <v>38</v>
       </c>
       <c r="C40" s="15" t="s">
@@ -18112,11 +18242,11 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="19">
-        <v>0</v>
-      </c>
-      <c r="B41" s="19">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="14">
+        <v>0</v>
+      </c>
+      <c r="B41" s="14">
         <v>39</v>
       </c>
       <c r="C41" s="15" t="s">
@@ -18126,11 +18256,11 @@
         <v>871</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="19">
-        <v>0</v>
-      </c>
-      <c r="B42" s="19">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="14">
+        <v>0</v>
+      </c>
+      <c r="B42" s="14">
         <v>40</v>
       </c>
       <c r="C42" s="15" t="s">
@@ -18140,11 +18270,11 @@
         <v>872</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="19">
-        <v>0</v>
-      </c>
-      <c r="B43" s="19">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="14">
+        <v>0</v>
+      </c>
+      <c r="B43" s="14">
         <v>41</v>
       </c>
       <c r="C43" s="15" t="s">
@@ -18154,11 +18284,11 @@
         <v>873</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="19">
-        <v>0</v>
-      </c>
-      <c r="B44" s="19">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="14">
+        <v>0</v>
+      </c>
+      <c r="B44" s="14">
         <v>42</v>
       </c>
       <c r="C44" s="15" t="s">
@@ -18168,11 +18298,11 @@
         <v>874</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="19">
-        <v>0</v>
-      </c>
-      <c r="B45" s="19">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="14">
+        <v>0</v>
+      </c>
+      <c r="B45" s="14">
         <v>43</v>
       </c>
       <c r="C45" s="15" t="s">
@@ -18182,11 +18312,11 @@
         <v>875</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="19">
-        <v>0</v>
-      </c>
-      <c r="B46" s="19">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="14">
+        <v>0</v>
+      </c>
+      <c r="B46" s="14">
         <v>44</v>
       </c>
       <c r="C46" s="15" t="s">
@@ -18196,11 +18326,11 @@
         <v>876</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="19">
-        <v>0</v>
-      </c>
-      <c r="B47" s="19">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="14">
+        <v>0</v>
+      </c>
+      <c r="B47" s="14">
         <v>45</v>
       </c>
       <c r="C47" s="15" t="s">
@@ -18210,11 +18340,11 @@
         <v>877</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="19">
-        <v>0</v>
-      </c>
-      <c r="B48" s="19">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="14">
+        <v>0</v>
+      </c>
+      <c r="B48" s="14">
         <v>46</v>
       </c>
       <c r="C48" s="15" t="s">
@@ -18224,11 +18354,11 @@
         <v>878</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="19">
-        <v>0</v>
-      </c>
-      <c r="B49" s="19">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="14">
+        <v>0</v>
+      </c>
+      <c r="B49" s="14">
         <v>47</v>
       </c>
       <c r="C49" s="15" t="s">
@@ -18238,11 +18368,11 @@
         <v>879</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="19">
-        <v>0</v>
-      </c>
-      <c r="B50" s="19">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="14">
+        <v>0</v>
+      </c>
+      <c r="B50" s="14">
         <v>48</v>
       </c>
       <c r="C50" s="15" t="s">
@@ -18252,11 +18382,11 @@
         <v>880</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="19">
-        <v>0</v>
-      </c>
-      <c r="B51" s="19">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="14">
+        <v>0</v>
+      </c>
+      <c r="B51" s="14">
         <v>49</v>
       </c>
       <c r="C51" s="15" t="s">
@@ -18266,11 +18396,11 @@
         <v>881</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="19">
-        <v>0</v>
-      </c>
-      <c r="B52" s="19">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="14">
+        <v>0</v>
+      </c>
+      <c r="B52" s="14">
         <v>50</v>
       </c>
       <c r="C52" s="15" t="s">
@@ -18280,11 +18410,11 @@
         <v>882</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="19">
-        <v>0</v>
-      </c>
-      <c r="B53" s="19">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="14">
+        <v>0</v>
+      </c>
+      <c r="B53" s="14">
         <v>51</v>
       </c>
       <c r="C53" s="15" t="s">
@@ -18294,11 +18424,11 @@
         <v>883</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="19">
-        <v>0</v>
-      </c>
-      <c r="B54" s="19">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="14">
+        <v>0</v>
+      </c>
+      <c r="B54" s="14">
         <v>52</v>
       </c>
       <c r="C54" s="15" t="s">
@@ -18309,10 +18439,10 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="19">
-        <v>0</v>
-      </c>
-      <c r="B55" s="19">
+      <c r="A55" s="14">
+        <v>0</v>
+      </c>
+      <c r="B55" s="14">
         <v>53</v>
       </c>
       <c r="C55" s="15" t="s">
@@ -18323,10 +18453,10 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="19">
-        <v>0</v>
-      </c>
-      <c r="B56" s="19">
+      <c r="A56" s="14">
+        <v>0</v>
+      </c>
+      <c r="B56" s="14">
         <v>54</v>
       </c>
       <c r="C56" s="15" t="s">
@@ -18337,10 +18467,10 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="19">
-        <v>0</v>
-      </c>
-      <c r="B57" s="19">
+      <c r="A57" s="14">
+        <v>0</v>
+      </c>
+      <c r="B57" s="14">
         <v>55</v>
       </c>
       <c r="C57" s="15" t="s">
@@ -18350,11 +18480,11 @@
         <v>887</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="19">
-        <v>0</v>
-      </c>
-      <c r="B58" s="19">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="14">
+        <v>0</v>
+      </c>
+      <c r="B58" s="14">
         <v>56</v>
       </c>
       <c r="C58" s="15" t="s">
@@ -18364,11 +18494,11 @@
         <v>888</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="19">
-        <v>0</v>
-      </c>
-      <c r="B59" s="19">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="14">
+        <v>0</v>
+      </c>
+      <c r="B59" s="14">
         <v>57</v>
       </c>
       <c r="C59" s="15" t="s">
@@ -18378,11 +18508,11 @@
         <v>889</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="19">
-        <v>0</v>
-      </c>
-      <c r="B60" s="19">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="14">
+        <v>0</v>
+      </c>
+      <c r="B60" s="14">
         <v>58</v>
       </c>
       <c r="C60" s="15" t="s">
@@ -18392,11 +18522,11 @@
         <v>890</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="19">
-        <v>0</v>
-      </c>
-      <c r="B61" s="19">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="14">
+        <v>0</v>
+      </c>
+      <c r="B61" s="14">
         <v>59</v>
       </c>
       <c r="C61" s="15" t="s">
@@ -18406,11 +18536,11 @@
         <v>891</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="19">
-        <v>0</v>
-      </c>
-      <c r="B62" s="19">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="14">
+        <v>0</v>
+      </c>
+      <c r="B62" s="14">
         <v>60</v>
       </c>
       <c r="C62" s="15" t="s">
@@ -18420,11 +18550,11 @@
         <v>892</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="19">
-        <v>0</v>
-      </c>
-      <c r="B63" s="19">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="14">
+        <v>0</v>
+      </c>
+      <c r="B63" s="14">
         <v>61</v>
       </c>
       <c r="C63" s="15" t="s">
@@ -18434,11 +18564,11 @@
         <v>893</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="19">
-        <v>0</v>
-      </c>
-      <c r="B64" s="19">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="14">
+        <v>0</v>
+      </c>
+      <c r="B64" s="14">
         <v>62</v>
       </c>
       <c r="C64" s="15" t="s">
@@ -18448,11 +18578,11 @@
         <v>894</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="19">
-        <v>0</v>
-      </c>
-      <c r="B65" s="19">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="14">
+        <v>0</v>
+      </c>
+      <c r="B65" s="14">
         <v>63</v>
       </c>
       <c r="C65" s="15" t="s">
@@ -18462,11 +18592,11 @@
         <v>895</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="19">
-        <v>0</v>
-      </c>
-      <c r="B66" s="19">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="14">
+        <v>0</v>
+      </c>
+      <c r="B66" s="14">
         <v>64</v>
       </c>
       <c r="C66" s="15" t="s">
@@ -18476,11 +18606,11 @@
         <v>896</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="19">
-        <v>0</v>
-      </c>
-      <c r="B67" s="19">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="14">
+        <v>0</v>
+      </c>
+      <c r="B67" s="14">
         <v>65</v>
       </c>
       <c r="C67" s="15" t="s">
@@ -18490,11 +18620,11 @@
         <v>422</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="19">
-        <v>0</v>
-      </c>
-      <c r="B68" s="19">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="14">
+        <v>0</v>
+      </c>
+      <c r="B68" s="14">
         <v>66</v>
       </c>
       <c r="C68" s="15" t="s">
@@ -18504,11 +18634,11 @@
         <v>509</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="19">
-        <v>0</v>
-      </c>
-      <c r="B69" s="19">
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="14">
+        <v>0</v>
+      </c>
+      <c r="B69" s="14">
         <v>67</v>
       </c>
       <c r="C69" s="15" t="s">
@@ -18518,11 +18648,11 @@
         <v>510</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="19">
-        <v>0</v>
-      </c>
-      <c r="B70" s="19">
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="14">
+        <v>0</v>
+      </c>
+      <c r="B70" s="14">
         <v>68</v>
       </c>
       <c r="C70" s="15" t="s">
@@ -18532,11 +18662,11 @@
         <v>419</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="19">
-        <v>0</v>
-      </c>
-      <c r="B71" s="19">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="14">
+        <v>0</v>
+      </c>
+      <c r="B71" s="14">
         <v>69</v>
       </c>
       <c r="C71" s="15" t="s">
@@ -18546,11 +18676,11 @@
         <v>511</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="19">
-        <v>0</v>
-      </c>
-      <c r="B72" s="19">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="14">
+        <v>0</v>
+      </c>
+      <c r="B72" s="14">
         <v>70</v>
       </c>
       <c r="C72" s="15" t="s">
@@ -18560,11 +18690,11 @@
         <v>512</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="19">
-        <v>0</v>
-      </c>
-      <c r="B73" s="19">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="14">
+        <v>0</v>
+      </c>
+      <c r="B73" s="14">
         <v>71</v>
       </c>
       <c r="C73" s="15" t="s">
@@ -18574,11 +18704,11 @@
         <v>421</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="19">
-        <v>0</v>
-      </c>
-      <c r="B74" s="19">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="14">
+        <v>0</v>
+      </c>
+      <c r="B74" s="14">
         <v>72</v>
       </c>
       <c r="C74" s="15" t="s">
@@ -18588,11 +18718,11 @@
         <v>515</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="19">
-        <v>0</v>
-      </c>
-      <c r="B75" s="19">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="14">
+        <v>0</v>
+      </c>
+      <c r="B75" s="14">
         <v>73</v>
       </c>
       <c r="C75" s="15" t="s">
@@ -18602,11 +18732,11 @@
         <v>516</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="19">
-        <v>0</v>
-      </c>
-      <c r="B76" s="19">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="14">
+        <v>0</v>
+      </c>
+      <c r="B76" s="14">
         <v>74</v>
       </c>
       <c r="C76" s="15" t="s">
@@ -18616,11 +18746,11 @@
         <v>420</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="19">
-        <v>0</v>
-      </c>
-      <c r="B77" s="19">
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="14">
+        <v>0</v>
+      </c>
+      <c r="B77" s="14">
         <v>75</v>
       </c>
       <c r="C77" s="15" t="s">
@@ -18630,11 +18760,11 @@
         <v>513</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="19">
-        <v>0</v>
-      </c>
-      <c r="B78" s="19">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="14">
+        <v>0</v>
+      </c>
+      <c r="B78" s="14">
         <v>76</v>
       </c>
       <c r="C78" s="15" t="s">
@@ -18645,10 +18775,10 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="19">
-        <v>0</v>
-      </c>
-      <c r="B79" s="19">
+      <c r="A79" s="14">
+        <v>0</v>
+      </c>
+      <c r="B79" s="14">
         <v>77</v>
       </c>
       <c r="C79" s="15" t="s">
@@ -18659,10 +18789,10 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="19">
-        <v>0</v>
-      </c>
-      <c r="B80" s="19">
+      <c r="A80" s="14">
+        <v>0</v>
+      </c>
+      <c r="B80" s="14">
         <v>78</v>
       </c>
       <c r="C80" s="15" t="s">
@@ -18673,10 +18803,10 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="19">
-        <v>0</v>
-      </c>
-      <c r="B81" s="19">
+      <c r="A81" s="14">
+        <v>0</v>
+      </c>
+      <c r="B81" s="14">
         <v>79</v>
       </c>
       <c r="C81" s="15" t="s">
@@ -18686,11 +18816,11 @@
         <v>518</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="19">
-        <v>0</v>
-      </c>
-      <c r="B82" s="19">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="14">
+        <v>0</v>
+      </c>
+      <c r="B82" s="14">
         <v>80</v>
       </c>
       <c r="C82" s="15" t="s">
@@ -18700,11 +18830,11 @@
         <v>897</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="19">
-        <v>0</v>
-      </c>
-      <c r="B83" s="19">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="14">
+        <v>0</v>
+      </c>
+      <c r="B83" s="14">
         <v>81</v>
       </c>
       <c r="C83" s="15" t="s">
@@ -18714,11 +18844,11 @@
         <v>898</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="19">
-        <v>0</v>
-      </c>
-      <c r="B84" s="19">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="14">
+        <v>0</v>
+      </c>
+      <c r="B84" s="14">
         <v>82</v>
       </c>
       <c r="C84" s="15" t="s">
@@ -18728,11 +18858,11 @@
         <v>473</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="19">
-        <v>0</v>
-      </c>
-      <c r="B85" s="19">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="14">
+        <v>0</v>
+      </c>
+      <c r="B85" s="14">
         <v>83</v>
       </c>
       <c r="C85" s="15" t="s">
@@ -18742,11 +18872,11 @@
         <v>474</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="19">
-        <v>0</v>
-      </c>
-      <c r="B86" s="19">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="14">
+        <v>0</v>
+      </c>
+      <c r="B86" s="14">
         <v>84</v>
       </c>
       <c r="C86" s="15" t="s">
@@ -18990,6 +19120,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EA9C388-CAA3-4695-949F-77695C0C0468}">
   <dimension ref="A1:D2"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.75" style="15" customWidth="1"/>
+    <col min="2" max="2" width="9.25" style="15" customWidth="1"/>
+    <col min="3" max="3" width="13.125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="19" style="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="14">
+        <v>0</v>
+      </c>
+      <c r="B2" s="14">
+        <v>0</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F23E19F-8F9E-49D0-AC0C-2A5018D314E9}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.75" style="15" customWidth="1"/>
+    <col min="2" max="2" width="9.25" style="15" customWidth="1"/>
+    <col min="3" max="3" width="13.125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="19" style="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="14">
+        <v>0</v>
+      </c>
+      <c r="B2" s="14">
+        <v>0</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53330EF9-A512-4EF3-B082-B966A8726E04}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>

</xml_diff>

<commit_message>
Add BlendMaterial (VRayBlendMtl && CoronaLayerMtl)
</commit_message>
<xml_diff>
--- a/RedHaloM2B_Lib/ParamBlock2/PB2.xlsx
+++ b/RedHaloM2B_Lib/ParamBlock2/PB2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APP\RedHaloM2B_Lib\RedHaloM2B_Lib\ParamBlock2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488B8F7C-59A1-47B7-83B3-25EA54CA37EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442A5ADC-C464-42D0-98B6-3CC2D37F08F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23160" yWindow="2265" windowWidth="27105" windowHeight="13710" tabRatio="706" firstSheet="28" activeTab="32" xr2:uid="{3B29243F-53F5-4745-B8C6-E4F7709AB902}"/>
+    <workbookView xWindow="18990" yWindow="2805" windowWidth="27105" windowHeight="13710" tabRatio="706" firstSheet="28" activeTab="34" xr2:uid="{3B29243F-53F5-4745-B8C6-E4F7709AB902}"/>
   </bookViews>
   <sheets>
     <sheet name="Checker" sheetId="6" r:id="rId1"/>
@@ -46,8 +46,8 @@
     <sheet name="Double Material" sheetId="33" r:id="rId31"/>
     <sheet name="VRayOverrideMtl" sheetId="34" r:id="rId32"/>
     <sheet name="CoronaRaySwitchMtl" sheetId="35" r:id="rId33"/>
-    <sheet name="Color Map (26)" sheetId="36" r:id="rId34"/>
-    <sheet name="Color Map (27)" sheetId="37" r:id="rId35"/>
+    <sheet name="VRayBlendMtl" sheetId="36" r:id="rId34"/>
+    <sheet name="CoronaLayerMtl" sheetId="37" r:id="rId35"/>
     <sheet name="Color Map (28)" sheetId="38" r:id="rId36"/>
   </sheets>
   <definedNames>
@@ -55,14 +55,13 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Checker!$A$3:$A$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Color Correction'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Color Map'!$A$2:$A$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="33" hidden="1">'Color Map (26)'!$A$2:$A$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="34" hidden="1">'Color Map (27)'!$A$2:$A$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="35" hidden="1">'Color Map (28)'!$A$2:$A$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">Composite!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">CoronaAO!$A$2:$A$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">CoronaBumpConverter!$A$2:$A$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">CoronaColorCorrect!$A$2:$A$32</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">CoronaFrontBack!$A$2:$A$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="34" hidden="1">CoronaLayerMtl!$A$2:$A$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">CoronaLegacyMtl!$A$2:$A$128</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="26" hidden="1">CoronaLightMtl!$A$2:$A$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">CoronaMix!$A$2:$A$16</definedName>
@@ -77,6 +76,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="27" hidden="1">StandardMtl!$A$2:$A$37</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="29" hidden="1">VRay2SidedMtl!$A$2:$A$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">VRayBitmap!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="33" hidden="1">VRayBlendMtl!$A$2:$A$45</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">VRayBump2Normal!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="28" hidden="1">VRayCarPaintMtl2!$A$2:$A$86</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">VRayColor!$A$2:$A$13</definedName>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2333" uniqueCount="928">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2435" uniqueCount="980">
   <si>
     <t>soften</t>
   </si>
@@ -2893,6 +2893,163 @@
   </si>
   <si>
     <t>directMtlOn</t>
+  </si>
+  <si>
+    <t>coatMtl_enable</t>
+  </si>
+  <si>
+    <t>MtlTab</t>
+  </si>
+  <si>
+    <t>coatMtl</t>
+  </si>
+  <si>
+    <t>RgbaTab</t>
+  </si>
+  <si>
+    <t>blend</t>
+  </si>
+  <si>
+    <t>texmap_blend</t>
+  </si>
+  <si>
+    <t>texmap_blend_multiplier</t>
+  </si>
+  <si>
+    <t>additiveMode</t>
+  </si>
+  <si>
+    <t>additiveDispl</t>
+  </si>
+  <si>
+    <t>coatMtl_0</t>
+  </si>
+  <si>
+    <t>blend_0</t>
+  </si>
+  <si>
+    <t>texmap_blend_0</t>
+  </si>
+  <si>
+    <t>texmap_blend_mult_0</t>
+  </si>
+  <si>
+    <t>coatMtl_1</t>
+  </si>
+  <si>
+    <t>blend_1</t>
+  </si>
+  <si>
+    <t>texmap_blend_1</t>
+  </si>
+  <si>
+    <t>texmap_blend_mult_1</t>
+  </si>
+  <si>
+    <t>coatMtl_2</t>
+  </si>
+  <si>
+    <t>blend_2</t>
+  </si>
+  <si>
+    <t>texmap_blend_2</t>
+  </si>
+  <si>
+    <t>texmap_blend_mult_2</t>
+  </si>
+  <si>
+    <t>coatMtl_3</t>
+  </si>
+  <si>
+    <t>blend_3</t>
+  </si>
+  <si>
+    <t>texmap_blend_3</t>
+  </si>
+  <si>
+    <t>texmap_blend_mult_3</t>
+  </si>
+  <si>
+    <t>coatMtl_4</t>
+  </si>
+  <si>
+    <t>blend_4</t>
+  </si>
+  <si>
+    <t>texmap_blend_4</t>
+  </si>
+  <si>
+    <t>texmap_blend_mult_4</t>
+  </si>
+  <si>
+    <t>coatMtl_5</t>
+  </si>
+  <si>
+    <t>blend_5</t>
+  </si>
+  <si>
+    <t>texmap_blend_5</t>
+  </si>
+  <si>
+    <t>texmap_blend_mult_5</t>
+  </si>
+  <si>
+    <t>coatMtl_6</t>
+  </si>
+  <si>
+    <t>blend_6</t>
+  </si>
+  <si>
+    <t>texmap_blend_6</t>
+  </si>
+  <si>
+    <t>texmap_blend_mult_6</t>
+  </si>
+  <si>
+    <t>coatMtl_7</t>
+  </si>
+  <si>
+    <t>blend_7</t>
+  </si>
+  <si>
+    <t>texmap_blend_7</t>
+  </si>
+  <si>
+    <t>texmap_blend_mult_7</t>
+  </si>
+  <si>
+    <t>coatMtl_8</t>
+  </si>
+  <si>
+    <t>blend_8</t>
+  </si>
+  <si>
+    <t>texmap_blend_8</t>
+  </si>
+  <si>
+    <t>texmap_blend_mult_8</t>
+  </si>
+  <si>
+    <t>layers</t>
+  </si>
+  <si>
+    <t>mixmaps</t>
+  </si>
+  <si>
+    <t>layersOn</t>
+  </si>
+  <si>
+    <t>masksOn</t>
+  </si>
+  <si>
+    <t>maskAmounts</t>
+  </si>
+  <si>
+    <t>displacementHandling</t>
+  </si>
+  <si>
+    <t>amounts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3100,7 +3257,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3156,9 +3313,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5567,8 +5721,8 @@
 </file>
 
 <file path=xl/tables/table34.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{72FB841A-FFF0-47DB-B2C0-A35A282F9844}" name="表6_8921213141516171819202122232425262728293031323335" displayName="表6_8921213141516171819202122232425262728293031323335" ref="A1:D2" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A1:D2" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{72FB841A-FFF0-47DB-B2C0-A35A282F9844}" name="表6_8921213141516171819202122232425262728293031323335" displayName="表6_8921213141516171819202122232425262728293031323335" ref="A1:D45" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:D45" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A04F6EBF-70EC-4FEE-96A7-0D91689FD415}" name="main" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{7C288209-724C-463E-9188-B7F0F00271FC}" name="branch" dataDxfId="14"/>
@@ -5580,8 +5734,8 @@
 </file>
 
 <file path=xl/tables/table35.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{CB340B27-1C4E-4F9E-A767-1DF332353E8B}" name="表6_892121314151617181920212223242526272829303132333536" displayName="表6_892121314151617181920212223242526272829303132333536" ref="A1:D2" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:D2" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{CB340B27-1C4E-4F9E-A767-1DF332353E8B}" name="表6_892121314151617181920212223242526272829303132333536" displayName="表6_892121314151617181920212223242526272829303132333536" ref="A1:D10" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:D10" xr:uid="{CECEF44C-6E82-4E17-A545-F55BBAAA3343}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{537BDF6A-461F-40A5-8C51-9B9DF4BA908E}" name="main" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{FBDC3124-FC59-4874-9202-8DAB5C2D1D04}" name="branch" dataDxfId="8"/>
@@ -19740,7 +19894,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -19780,10 +19934,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="19">
-        <v>0</v>
-      </c>
-      <c r="B3" s="19">
+      <c r="A3" s="14">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14">
         <v>1</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -19794,10 +19948,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="19">
-        <v>0</v>
-      </c>
-      <c r="B4" s="19">
+      <c r="A4" s="14">
+        <v>0</v>
+      </c>
+      <c r="B4" s="14">
         <v>2</v>
       </c>
       <c r="C4" s="15" t="s">
@@ -19808,10 +19962,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="19">
-        <v>0</v>
-      </c>
-      <c r="B5" s="19">
+      <c r="A5" s="14">
+        <v>0</v>
+      </c>
+      <c r="B5" s="14">
         <v>3</v>
       </c>
       <c r="C5" s="15" t="s">
@@ -19822,10 +19976,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="19">
-        <v>0</v>
-      </c>
-      <c r="B6" s="19">
+      <c r="A6" s="14">
+        <v>0</v>
+      </c>
+      <c r="B6" s="14">
         <v>4</v>
       </c>
       <c r="C6" s="15" t="s">
@@ -19836,10 +19990,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="19">
-        <v>0</v>
-      </c>
-      <c r="B7" s="19">
+      <c r="A7" s="14">
+        <v>0</v>
+      </c>
+      <c r="B7" s="14">
         <v>5</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -19850,10 +20004,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="19">
-        <v>0</v>
-      </c>
-      <c r="B8" s="19">
+      <c r="A8" s="14">
+        <v>0</v>
+      </c>
+      <c r="B8" s="14">
         <v>6</v>
       </c>
       <c r="C8" s="15" t="s">
@@ -19864,10 +20018,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="19">
-        <v>0</v>
-      </c>
-      <c r="B9" s="19">
+      <c r="A9" s="14">
+        <v>0</v>
+      </c>
+      <c r="B9" s="14">
         <v>7</v>
       </c>
       <c r="C9" s="15" t="s">
@@ -19878,10 +20032,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="19">
-        <v>0</v>
-      </c>
-      <c r="B10" s="19">
+      <c r="A10" s="14">
+        <v>0</v>
+      </c>
+      <c r="B10" s="14">
         <v>8</v>
       </c>
       <c r="C10" s="15" t="s">
@@ -19892,10 +20046,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="19">
-        <v>0</v>
-      </c>
-      <c r="B11" s="19">
+      <c r="A11" s="14">
+        <v>0</v>
+      </c>
+      <c r="B11" s="14">
         <v>9</v>
       </c>
       <c r="C11" s="15" t="s">
@@ -19918,8 +20072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9947EFD0-D125-41D4-A27D-AF130832AA7F}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -19959,10 +20113,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="19">
-        <v>0</v>
-      </c>
-      <c r="B3" s="19">
+      <c r="A3" s="14">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14">
         <v>1</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -19973,10 +20127,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="19">
-        <v>0</v>
-      </c>
-      <c r="B4" s="19">
+      <c r="A4" s="14">
+        <v>0</v>
+      </c>
+      <c r="B4" s="14">
         <v>2</v>
       </c>
       <c r="C4" s="15" t="s">
@@ -19987,10 +20141,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="19">
-        <v>0</v>
-      </c>
-      <c r="B5" s="19">
+      <c r="A5" s="14">
+        <v>0</v>
+      </c>
+      <c r="B5" s="14">
         <v>3</v>
       </c>
       <c r="C5" s="15" t="s">
@@ -20001,10 +20155,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="19">
-        <v>0</v>
-      </c>
-      <c r="B6" s="19">
+      <c r="A6" s="14">
+        <v>0</v>
+      </c>
+      <c r="B6" s="14">
         <v>4</v>
       </c>
       <c r="C6" s="15" t="s">
@@ -20015,10 +20169,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="19">
-        <v>0</v>
-      </c>
-      <c r="B7" s="19">
+      <c r="A7" s="14">
+        <v>0</v>
+      </c>
+      <c r="B7" s="14">
         <v>5</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -20029,10 +20183,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="19">
-        <v>0</v>
-      </c>
-      <c r="B8" s="19">
+      <c r="A8" s="14">
+        <v>0</v>
+      </c>
+      <c r="B8" s="14">
         <v>6</v>
       </c>
       <c r="C8" s="15" t="s">
@@ -20043,10 +20197,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="19">
-        <v>0</v>
-      </c>
-      <c r="B9" s="19">
+      <c r="A9" s="14">
+        <v>0</v>
+      </c>
+      <c r="B9" s="14">
         <v>7</v>
       </c>
       <c r="C9" s="15" t="s">
@@ -20057,10 +20211,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="19">
-        <v>0</v>
-      </c>
-      <c r="B10" s="19">
+      <c r="A10" s="14">
+        <v>0</v>
+      </c>
+      <c r="B10" s="14">
         <v>8</v>
       </c>
       <c r="C10" s="15" t="s">
@@ -20071,10 +20225,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="19">
-        <v>0</v>
-      </c>
-      <c r="B11" s="19">
+      <c r="A11" s="14">
+        <v>0</v>
+      </c>
+      <c r="B11" s="14">
         <v>9</v>
       </c>
       <c r="C11" s="15" t="s">
@@ -20095,10 +20249,10 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1EAC900-1657-4514-B3AC-81D86DD6161A}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -20106,7 +20260,7 @@
     <col min="1" max="1" width="9.75" style="15" customWidth="1"/>
     <col min="2" max="2" width="9.25" style="15" customWidth="1"/>
     <col min="3" max="3" width="13.125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="19" style="15" customWidth="1"/>
+    <col min="4" max="4" width="22.625" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
@@ -20131,10 +20285,612 @@
         <v>0</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>62</v>
+        <v>899</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>120</v>
+        <v>911</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="14">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="14">
+        <v>0</v>
+      </c>
+      <c r="B4" s="14">
+        <v>2</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>929</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="14">
+        <v>0</v>
+      </c>
+      <c r="B5" s="14">
+        <v>3</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>931</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="14">
+        <v>0</v>
+      </c>
+      <c r="B6" s="14">
+        <v>4</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>321</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="14">
+        <v>0</v>
+      </c>
+      <c r="B7" s="14">
+        <v>5</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="14">
+        <v>0</v>
+      </c>
+      <c r="B8" s="14">
+        <v>6</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="14">
+        <v>0</v>
+      </c>
+      <c r="B9" s="14">
+        <v>7</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="14">
+        <v>0</v>
+      </c>
+      <c r="B10" s="14">
+        <v>8</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>899</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="14">
+        <v>0</v>
+      </c>
+      <c r="B11" s="14">
+        <v>9</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="14">
+        <v>0</v>
+      </c>
+      <c r="B12" s="14">
+        <v>10</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="14">
+        <v>0</v>
+      </c>
+      <c r="B13" s="14">
+        <v>11</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="14">
+        <v>0</v>
+      </c>
+      <c r="B14" s="14">
+        <v>12</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>899</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="14">
+        <v>0</v>
+      </c>
+      <c r="B15" s="14">
+        <v>13</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="14">
+        <v>0</v>
+      </c>
+      <c r="B16" s="14">
+        <v>14</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="14">
+        <v>0</v>
+      </c>
+      <c r="B17" s="14">
+        <v>15</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="14">
+        <v>0</v>
+      </c>
+      <c r="B18" s="14">
+        <v>16</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>899</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="14">
+        <v>0</v>
+      </c>
+      <c r="B19" s="14">
+        <v>17</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="14">
+        <v>0</v>
+      </c>
+      <c r="B20" s="14">
+        <v>18</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="14">
+        <v>0</v>
+      </c>
+      <c r="B21" s="14">
+        <v>19</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="14">
+        <v>0</v>
+      </c>
+      <c r="B22" s="14">
+        <v>20</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>899</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="14">
+        <v>0</v>
+      </c>
+      <c r="B23" s="14">
+        <v>21</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="14">
+        <v>0</v>
+      </c>
+      <c r="B24" s="14">
+        <v>22</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="14">
+        <v>0</v>
+      </c>
+      <c r="B25" s="14">
+        <v>23</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="14">
+        <v>0</v>
+      </c>
+      <c r="B26" s="14">
+        <v>24</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>899</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="14">
+        <v>0</v>
+      </c>
+      <c r="B27" s="14">
+        <v>25</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="14">
+        <v>0</v>
+      </c>
+      <c r="B28" s="14">
+        <v>26</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="14">
+        <v>0</v>
+      </c>
+      <c r="B29" s="14">
+        <v>27</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="14">
+        <v>0</v>
+      </c>
+      <c r="B30" s="14">
+        <v>28</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>899</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="14">
+        <v>0</v>
+      </c>
+      <c r="B31" s="14">
+        <v>29</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="14">
+        <v>0</v>
+      </c>
+      <c r="B32" s="14">
+        <v>30</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="14">
+        <v>0</v>
+      </c>
+      <c r="B33" s="14">
+        <v>31</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="14">
+        <v>0</v>
+      </c>
+      <c r="B34" s="14">
+        <v>32</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>899</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="14">
+        <v>0</v>
+      </c>
+      <c r="B35" s="14">
+        <v>33</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="14">
+        <v>0</v>
+      </c>
+      <c r="B36" s="14">
+        <v>34</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="14">
+        <v>0</v>
+      </c>
+      <c r="B37" s="14">
+        <v>35</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="14">
+        <v>0</v>
+      </c>
+      <c r="B38" s="14">
+        <v>36</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>899</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="14">
+        <v>0</v>
+      </c>
+      <c r="B39" s="14">
+        <v>37</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="14">
+        <v>0</v>
+      </c>
+      <c r="B40" s="14">
+        <v>38</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="14">
+        <v>0</v>
+      </c>
+      <c r="B41" s="14">
+        <v>39</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="14">
+        <v>0</v>
+      </c>
+      <c r="B42" s="14">
+        <v>40</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>899</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="14">
+        <v>0</v>
+      </c>
+      <c r="B43" s="14">
+        <v>41</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="14">
+        <v>0</v>
+      </c>
+      <c r="B44" s="14">
+        <v>42</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="14">
+        <v>0</v>
+      </c>
+      <c r="B45" s="14">
+        <v>43</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>972</v>
       </c>
     </row>
   </sheetData>
@@ -20148,10 +20904,10 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F3110F0-2F63-49D3-B561-F4C18DBAA044}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -20159,7 +20915,7 @@
     <col min="1" max="1" width="9.75" style="15" customWidth="1"/>
     <col min="2" max="2" width="9.25" style="15" customWidth="1"/>
     <col min="3" max="3" width="13.125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="19" style="15" customWidth="1"/>
+    <col min="4" max="4" width="20.625" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
@@ -20184,10 +20940,122 @@
         <v>0</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>62</v>
+        <v>899</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>120</v>
+        <v>911</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="14">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>929</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="14">
+        <v>0</v>
+      </c>
+      <c r="B4" s="14">
+        <v>2</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>321</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="14">
+        <v>0</v>
+      </c>
+      <c r="B5" s="14">
+        <v>3</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="14">
+        <v>0</v>
+      </c>
+      <c r="B6" s="14">
+        <v>4</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="14">
+        <v>0</v>
+      </c>
+      <c r="B7" s="14">
+        <v>5</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="14">
+        <v>0</v>
+      </c>
+      <c r="B8" s="14">
+        <v>6</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="14">
+        <v>0</v>
+      </c>
+      <c r="B9" s="14">
+        <v>7</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="14">
+        <v>0</v>
+      </c>
+      <c r="B10" s="14">
+        <v>8</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>